<commit_message>
Changed Interview Import Me Header.csv
</commit_message>
<xml_diff>
--- a/OPID/Uploads/Voided Checks September  2017.xlsx
+++ b/OPID/Uploads/Voided Checks September  2017.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21975" windowHeight="7125" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
   <si>
     <t>Date of Check</t>
   </si>
@@ -274,6 +274,27 @@
   </si>
   <si>
     <t>80522</t>
+  </si>
+  <si>
+    <t>81684</t>
+  </si>
+  <si>
+    <t>81806</t>
+  </si>
+  <si>
+    <t>81314</t>
+  </si>
+  <si>
+    <t>81234</t>
+  </si>
+  <si>
+    <t>81305</t>
+  </si>
+  <si>
+    <t>81857</t>
+  </si>
+  <si>
+    <t>81125</t>
   </si>
 </sst>
 </file>
@@ -641,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G127"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A85" sqref="A85"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1640,39 +1661,67 @@
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="6"/>
+      <c r="A85" s="6">
+        <v>42992</v>
+      </c>
       <c r="B85" s="1"/>
-      <c r="C85" s="7"/>
+      <c r="C85" s="7" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="6"/>
+      <c r="A86" s="6">
+        <v>42999</v>
+      </c>
       <c r="B86" s="1"/>
-      <c r="C86" s="7"/>
+      <c r="C86" s="7" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="6"/>
+      <c r="A87" s="6">
+        <v>42990</v>
+      </c>
       <c r="B87" s="1"/>
-      <c r="C87" s="7"/>
+      <c r="C87" s="7" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="6"/>
+      <c r="A88" s="6">
+        <v>42992</v>
+      </c>
       <c r="B88" s="1"/>
-      <c r="C88" s="7"/>
+      <c r="C88" s="7" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="6"/>
+      <c r="A89" s="6">
+        <v>42948</v>
+      </c>
       <c r="B89" s="1"/>
-      <c r="C89" s="7"/>
+      <c r="C89" s="7" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="6"/>
+      <c r="A90" s="6">
+        <v>43034</v>
+      </c>
       <c r="B90" s="1"/>
-      <c r="C90" s="7"/>
+      <c r="C90" s="7" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="6"/>
+      <c r="A91" s="6">
+        <v>42964</v>
+      </c>
       <c r="B91" s="1"/>
-      <c r="C91" s="7"/>
+      <c r="C91" s="7" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="6"/>

</xml_diff>